<commit_message>
Atualização automática de BENTO_GONCALVES.xlsx
</commit_message>
<xml_diff>
--- a/BENTO_GONCALVES.xlsx
+++ b/BENTO_GONCALVES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8C11A97-7E97-4B4B-9C9C-E70E25561912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{713C074B-BB2F-4C9C-8B2F-1C91A473F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,20 +24,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="8" r:id="rId9"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1271,7 +1258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1332,30 +1319,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1373,7 +1336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1412,17 +1375,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1474,7 +1432,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{9A56818E-DDAF-4285-A7AB-08A45DBDAD76}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{26477103-4F33-4CB9-B291-0E5F2FEA2D31}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1504,10 +1462,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B935212-191D-4357-8979-A4A79B0E7381}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF403A97-B2D0-42DC-980D-6D1CF4229ABF}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1545,7 +1503,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09EB24EB-3FA5-4364-9854-5AE4B15830C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{250AEB02-333C-4163-AAEE-F3BCE767C8F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1608,7 +1566,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C867A8-E349-4AB2-ACB1-07E7120FBB21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6344D98A-85D1-4964-94C8-6223F61E9CFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1627,7 +1585,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3E2ABF-E3A8-6917-9E90-A7002C0682F6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9E5654-DB42-AD8B-E22D-0F8651CF6307}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1676,7 +1634,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD5A1D4-1DAC-E96F-AD6A-98FCCEDA98CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6D007C6-7D23-951F-65B0-142A7D98103A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1695,7 +1653,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D2E09B-4962-AB58-40FE-A2FD74F198A1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09C9D63B-C8D8-D219-1886-686F02D07CAA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1726,7 +1684,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D9EFE71-67DB-E3DE-6BC0-87652D3DED9D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14DC7B3A-C53C-BED1-EFCD-D181D558CE04}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1757,7 +1715,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B979AF4-DCE7-5C21-8F09-DBD2FCED2B37}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6096F6A6-3B1B-53E9-D0B0-6ABAF123F86A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1800,7 +1758,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F3760B6-0CD5-487B-BFB5-366136C36C59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C69E3556-C69C-4608-BE5F-3256094A1DFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1838,7 +1796,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A0D172-B202-4F5B-A467-C2859E77B3FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A78AAD2B-3BBA-4AEF-871A-D7D24A2258A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1881,7 +1839,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77F675E3-2F8B-49D9-A497-D8D110B9092F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{518675E0-9327-4DAD-9A5F-86C62B2B3035}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2194,7 +2152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045AF7D6-81EF-4183-8331-79E41D778301}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1117CE6-9242-4DEE-B900-2EA2B32F1745}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2206,98 +2164,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="42"/>
-    <col min="6" max="6" width="2" style="42" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="42" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="42"/>
+    <col min="1" max="5" width="12.5703125" style="39"/>
+    <col min="6" max="6" width="2" style="39" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="39" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="41"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="41"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="41"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="41"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="41"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="41"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="41"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="41"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="41"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="41"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="41"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="41"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="41"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="41"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="41"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="41"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="41"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="41"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="41"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="41"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="41"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="41"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="41"/>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="41"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="41"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="41"/>
+      <c r="F26" s="38"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="41"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="41"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="41"/>
+      <c r="F29" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -2327,25 +2285,24 @@
       <c r="B1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="33" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="37">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="34">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="37">
         <v>62</v>
       </c>
-      <c r="F1" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="B2" s="40">
-        <v>62</v>
-      </c>
-      <c r="C2" s="38">
+      <c r="C2" s="35">
         <v>4.0999867742362124E-3</v>
       </c>
     </row>
@@ -5610,19 +5567,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5656,46 +5613,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5703,7 +5660,7 @@
       <c r="A2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>241342</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5715,10 +5672,10 @@
       <c r="E2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>22.4</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>224</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5747,7 +5704,7 @@
       <c r="A3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>241395</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5759,10 +5716,10 @@
       <c r="E3" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>20.6</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>206</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5791,7 +5748,7 @@
       <c r="A4" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>415921</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5803,10 +5760,10 @@
       <c r="E4" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>36.700000000000003</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>367</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5835,7 +5792,7 @@
       <c r="A5" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>437181</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5847,10 +5804,10 @@
       <c r="E5" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>36.53</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>365.25</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5889,14 +5846,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>299</v>
       </c>
     </row>
@@ -5927,46 +5884,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5984,16 +5941,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6027,7 +5984,7 @@
       <c r="J1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6041,10 +5998,10 @@
       <c r="C2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="20">
         <v>1282</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="20">
         <v>128.19999999999999</v>
       </c>
       <c r="F2" s="2">
@@ -6062,7 +6019,7 @@
       <c r="J2" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="K2" s="28">
+      <c r="K2" s="25">
         <v>9878</v>
       </c>
     </row>
@@ -6076,10 +6033,10 @@
       <c r="C3" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="20">
         <v>70</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="20">
         <v>7</v>
       </c>
       <c r="F3" s="2">
@@ -6097,7 +6054,7 @@
       <c r="J3" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K3" s="28">
+      <c r="K3" s="25">
         <v>17546</v>
       </c>
     </row>
@@ -6111,10 +6068,10 @@
       <c r="C4" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <v>45</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="20">
         <v>4.5</v>
       </c>
       <c r="F4" s="2">
@@ -6132,7 +6089,7 @@
       <c r="J4" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="25">
         <v>655</v>
       </c>
     </row>
@@ -6146,10 +6103,10 @@
       <c r="C5" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>45</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>4.5</v>
       </c>
       <c r="F5" s="2">
@@ -6167,7 +6124,7 @@
       <c r="J5" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="25">
         <v>14476</v>
       </c>
     </row>
@@ -6181,10 +6138,10 @@
       <c r="C6" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>100</v>
       </c>
       <c r="F6" s="2">
@@ -6202,7 +6159,7 @@
       <c r="J6" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="25">
         <v>9692</v>
       </c>
     </row>
@@ -6216,10 +6173,10 @@
       <c r="C7" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>387.5</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>38.75</v>
       </c>
       <c r="F7" s="2">
@@ -6237,7 +6194,7 @@
       <c r="J7" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="25">
         <v>13868</v>
       </c>
     </row>
@@ -6251,10 +6208,10 @@
       <c r="C8" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>387.5</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>38.75</v>
       </c>
       <c r="F8" s="2">
@@ -6272,7 +6229,7 @@
       <c r="J8" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="25">
         <v>13868</v>
       </c>
     </row>
@@ -6286,10 +6243,10 @@
       <c r="C9" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>185</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <v>18.5</v>
       </c>
       <c r="F9" s="2">
@@ -6307,7 +6264,7 @@
       <c r="J9" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="25">
         <v>18567</v>
       </c>
     </row>
@@ -6321,10 +6278,10 @@
       <c r="C10" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>221</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>22.1</v>
       </c>
       <c r="F10" s="2">
@@ -6342,7 +6299,7 @@
       <c r="J10" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="25">
         <v>1084</v>
       </c>
     </row>
@@ -6356,10 +6313,10 @@
       <c r="C11" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <v>5357</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>535.70000000000005</v>
       </c>
       <c r="F11" s="2">
@@ -6377,7 +6334,7 @@
       <c r="J11" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="25">
         <v>18211</v>
       </c>
     </row>
@@ -6391,10 +6348,10 @@
       <c r="C12" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>6498.11</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>649.80999999999995</v>
       </c>
       <c r="F12" s="2">
@@ -6412,7 +6369,7 @@
       <c r="J12" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="25">
         <v>17546</v>
       </c>
     </row>
@@ -6426,10 +6383,10 @@
       <c r="C13" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="20">
         <v>3103.74</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <v>310.37</v>
       </c>
       <c r="F13" s="2">
@@ -6447,7 +6404,7 @@
       <c r="J13" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="25">
         <v>17546</v>
       </c>
     </row>
@@ -6461,10 +6418,10 @@
       <c r="C14" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="20">
         <v>3103.74</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="20">
         <v>310.37</v>
       </c>
       <c r="F14" s="2">
@@ -6482,7 +6439,7 @@
       <c r="J14" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="25">
         <v>17546</v>
       </c>
     </row>
@@ -6496,10 +6453,10 @@
       <c r="C15" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="20">
         <v>9205.2000000000007</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="20">
         <v>920.52</v>
       </c>
       <c r="F15" s="2">
@@ -6517,7 +6474,7 @@
       <c r="J15" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="25">
         <v>17546</v>
       </c>
     </row>
@@ -6531,10 +6488,10 @@
       <c r="C16" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="20">
         <v>216.87</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="20">
         <v>21.69</v>
       </c>
       <c r="F16" s="2">
@@ -6552,7 +6509,7 @@
       <c r="J16" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="25">
         <v>18092</v>
       </c>
     </row>
@@ -6566,10 +6523,10 @@
       <c r="C17" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="20">
         <v>345</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="20">
         <v>34.5</v>
       </c>
       <c r="F17" s="2">
@@ -6587,7 +6544,7 @@
       <c r="J17" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="25">
         <v>18092</v>
       </c>
     </row>
@@ -6601,10 +6558,10 @@
       <c r="C18" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="20">
         <v>5370.85</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="20">
         <v>537.09</v>
       </c>
       <c r="F18" s="2">
@@ -6622,7 +6579,7 @@
       <c r="J18" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="25">
         <v>19106</v>
       </c>
     </row>
@@ -6636,10 +6593,10 @@
       <c r="C19" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="20">
         <v>487.6</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="20">
         <v>132.63999999999999</v>
       </c>
       <c r="F19" s="2">
@@ -6657,7 +6614,7 @@
       <c r="J19" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K19" s="25">
         <v>17546</v>
       </c>
     </row>
@@ -6671,10 +6628,10 @@
       <c r="C20" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="20">
         <v>2662.07</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="20">
         <v>2202.9899999999998</v>
       </c>
       <c r="F20" s="2">
@@ -6692,7 +6649,7 @@
       <c r="J20" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20" s="25">
         <v>9604</v>
       </c>
     </row>
@@ -6717,54 +6674,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>349</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="27" t="s">
         <v>350</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="28" t="s">
         <v>353</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="26" t="s">
         <v>356</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="26" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6775,41 +6733,41 @@
       <c r="B2" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="29">
         <v>45901</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="30">
         <v>29602</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="30">
         <v>3771</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="32" t="s">
         <v>365</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="32" t="s">
         <v>365</v>
       </c>
     </row>

</xml_diff>